<commit_message>
Fixed Issue with Custom tool tip in line chart
</commit_message>
<xml_diff>
--- a/backend/expense_details.xlsx
+++ b/backend/expense_details.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -460,13 +460,13 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Rent</v>
+        <v>Video Games</v>
       </c>
       <c r="B6">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C6" s="1">
-        <v>45901.16680555556</v>
+        <v>45924.16680555556</v>
       </c>
     </row>
     <row r="7">
@@ -477,12 +477,23 @@
         <v>300</v>
       </c>
       <c r="C7" s="1">
+        <v>45901.16680555556</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Rent</v>
+      </c>
+      <c r="B8">
+        <v>300</v>
+      </c>
+      <c r="C8" s="1">
         <v>45689.16680555556</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>